<commit_message>
Added original working template of Budget_Dashboard.xlsx
</commit_message>
<xml_diff>
--- a/Projects/Budget_Dashboard/Budget_Dasboard.xlsx
+++ b/Projects/Budget_Dashboard/Budget_Dasboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\DADS\GitHub_Repositories\Excel\Projects\Budget_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD2BB837-96CE-4A30-8758-C7DF01187808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAA83EE-BE4B-451F-8AC4-97B8592A5DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{143A17CA-6C9C-4012-B34C-32BAD124D6AF}"/>
   </bookViews>
@@ -30,19 +30,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Settings</t>
   </si>
   <si>
     <t>General</t>
   </si>
+  <si>
+    <t>Starting Year:</t>
+  </si>
+  <si>
+    <t>Set the starting year (yyyy) once at the beginning and do not chnge again</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,8 +70,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,8 +105,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -88,8 +127,91 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color theme="1"/>
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -99,21 +221,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="1"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -121,18 +232,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -140,18 +240,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,16 +605,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B66AF2-6345-42B8-BD05-00FD95F37E66}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="3" width="1.89453125" customWidth="1"/>
-    <col min="4" max="7" width="16.68359375" customWidth="1"/>
+    <col min="4" max="6" width="16.68359375" customWidth="1"/>
+    <col min="7" max="7" width="50.7890625" customWidth="1"/>
     <col min="8" max="8" width="1.3125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -485,43 +625,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="2" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="4"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="16">
+        <v>2023</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" s="5"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="5"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C5:H5"/>
+  <mergeCells count="2">
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>